<commit_message>
Added description of the analysis
</commit_message>
<xml_diff>
--- a/src/team_4/tokens_dict.xlsx
+++ b/src/team_4/tokens_dict.xlsx
@@ -109,10 +109,10 @@
     <t xml:space="preserve">אין</t>
   </si>
   <si>
+    <t xml:space="preserve">אינו</t>
+  </si>
+  <si>
     <t xml:space="preserve">סבא</t>
-  </si>
-  <si>
-    <t xml:space="preserve">אינו</t>
   </si>
   <si>
     <t xml:space="preserve">מצבו</t>
@@ -2920,7 +2920,7 @@
   <dimension ref="A1:L645"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J55" activeCellId="0" sqref="J55"/>
+      <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3104,20 +3104,20 @@
       <c r="B8" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="9"/>
+      <c r="K8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="10" t="s">
@@ -3136,8 +3136,8 @@
       <c r="B10" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="K10" s="11" t="s">
         <v>33</v>
       </c>
@@ -3707,8 +3707,8 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="0"/>
-      <c r="D47" s="0"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="15" t="s">
@@ -3933,8 +3933,8 @@
       <c r="D61" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E61" s="0"/>
-      <c r="F61" s="0"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
       <c r="K61" s="15" t="s">
@@ -3945,8 +3945,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E62" s="0"/>
-      <c r="F62" s="0"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
       <c r="K62" s="15" t="s">
         <v>132</v>
       </c>
@@ -3961,8 +3961,8 @@
       <c r="B63" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E63" s="0"/>
-      <c r="F63" s="0"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
       <c r="K63" s="15" t="s">
         <v>134</v>
       </c>
@@ -4041,8 +4041,8 @@
       <c r="D68" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
       <c r="K68" s="15" t="s">
@@ -4203,8 +4203,6 @@
       </c>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
-      <c r="K78" s="0"/>
-      <c r="L78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="15" t="s">
@@ -4217,8 +4215,6 @@
       <c r="F79" s="14"/>
       <c r="I79" s="8"/>
       <c r="J79" s="8"/>
-      <c r="K79" s="0"/>
-      <c r="L79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="14" t="s">
@@ -4731,8 +4727,8 @@
       <c r="J134" s="8"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="0"/>
-      <c r="D135" s="0"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
       <c r="I135" s="8"/>
       <c r="J135" s="8"/>
     </row>
@@ -5277,8 +5273,8 @@
       <c r="J199" s="8"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="0"/>
-      <c r="D200" s="0"/>
+      <c r="C200" s="6"/>
+      <c r="D200" s="6"/>
       <c r="I200" s="8"/>
       <c r="J200" s="8"/>
     </row>
@@ -8429,8 +8425,8 @@
       <c r="D602" s="6"/>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C603" s="0"/>
-      <c r="D603" s="0"/>
+      <c r="C603" s="6"/>
+      <c r="D603" s="6"/>
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C604" s="15" t="s">

</xml_diff>

<commit_message>
Added categorization only 30 categories now
</commit_message>
<xml_diff>
--- a/src/team_4/tokens_dict.xlsx
+++ b/src/team_4/tokens_dict.xlsx
@@ -591,6 +591,9 @@
     <t xml:space="preserve">יועץ</t>
   </si>
   <si>
+    <t xml:space="preserve">האחרונה</t>
+  </si>
+  <si>
     <t xml:space="preserve">מכירות</t>
   </si>
   <si>
@@ -1765,9 +1768,6 @@
   </si>
   <si>
     <t xml:space="preserve">האמנות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">האחרונה</t>
   </si>
   <si>
     <t xml:space="preserve">האווירית</t>
@@ -2919,8 +2919,8 @@
   </sheetPr>
   <dimension ref="A1:L645"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O84" activeCellId="0" sqref="O84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3104,8 +3104,8 @@
       <c r="B8" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="13" t="s">
         <v>29</v>
       </c>
@@ -4203,10 +4203,16 @@
       </c>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
+      <c r="K78" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D79" s="2" t="n">
         <v>5</v>
@@ -4218,7 +4224,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F80" s="14" t="n">
         <v>5</v>
@@ -4226,7 +4232,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
       <c r="K80" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L80" s="3" t="n">
         <v>2</v>
@@ -4234,7 +4240,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D81" s="2" t="n">
         <v>5</v>
@@ -4248,7 +4254,7 @@
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F82" s="2" t="n">
         <v>5</v>
@@ -4258,7 +4264,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F83" s="3" t="n">
         <v>5</v>
@@ -4272,7 +4278,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D85" s="2" t="n">
         <v>5</v>
@@ -4282,7 +4288,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D86" s="2" t="n">
         <v>5</v>
@@ -4292,7 +4298,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B87" s="1" t="n">
         <v>5</v>
@@ -4302,7 +4308,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D88" s="2" t="n">
         <v>5</v>
@@ -4312,7 +4318,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D89" s="2" t="n">
         <v>4</v>
@@ -4322,7 +4328,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D90" s="2" t="n">
         <v>4</v>
@@ -4332,7 +4338,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B91" s="1" t="n">
         <v>4</v>
@@ -4342,7 +4348,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D92" s="2" t="n">
         <v>4</v>
@@ -4358,7 +4364,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D94" s="2" t="n">
         <v>4</v>
@@ -4368,7 +4374,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="15" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D95" s="2" t="n">
         <v>4</v>
@@ -4384,7 +4390,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F97" s="3" t="n">
         <v>4</v>
@@ -4394,7 +4400,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D98" s="2" t="n">
         <v>4</v>
@@ -4404,7 +4410,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D99" s="2" t="n">
         <v>4</v>
@@ -4414,7 +4420,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F100" s="3" t="n">
         <v>4</v>
@@ -4424,7 +4430,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F101" s="3" t="n">
         <v>4</v>
@@ -4438,7 +4444,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D103" s="2" t="n">
         <v>4</v>
@@ -4460,13 +4466,13 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D106" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F106" s="3" t="n">
         <v>4</v>
@@ -4476,7 +4482,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B107" s="1" t="n">
         <v>3</v>
@@ -4486,7 +4492,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D108" s="2" t="n">
         <v>3</v>
@@ -4496,7 +4502,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F109" s="3" t="n">
         <v>3</v>
@@ -4506,7 +4512,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D110" s="2" t="n">
         <v>3</v>
@@ -4516,7 +4522,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F111" s="3" t="n">
         <v>3</v>
@@ -4526,7 +4532,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D112" s="2" t="n">
         <v>3</v>
@@ -4536,7 +4542,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="14" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F113" s="3" t="n">
         <v>3</v>
@@ -4546,7 +4552,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F114" s="2" t="n">
         <v>3</v>
@@ -4554,7 +4560,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F115" s="3" t="n">
         <v>3</v>
@@ -4562,7 +4568,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D116" s="2" t="n">
         <v>3</v>
@@ -4570,7 +4576,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F117" s="3" t="n">
         <v>3</v>
@@ -4578,7 +4584,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="15" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D118" s="2" t="n">
         <v>3</v>
@@ -4586,7 +4592,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F119" s="3" t="n">
         <v>3</v>
@@ -4594,7 +4600,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F120" s="3" t="n">
         <v>3</v>
@@ -4602,7 +4608,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D121" s="2" t="n">
         <v>3</v>
@@ -4610,7 +4616,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="15" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D122" s="2" t="n">
         <v>3</v>
@@ -4622,7 +4628,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F124" s="2" t="n">
         <v>3</v>
@@ -4632,7 +4638,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B125" s="1" t="n">
         <v>3</v>
@@ -4642,7 +4648,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F126" s="3" t="n">
         <v>3</v>
@@ -4652,7 +4658,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D127" s="2" t="n">
         <v>3</v>
@@ -4663,7 +4669,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D128" s="2" t="n">
         <v>3</v>
@@ -4673,7 +4679,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="15" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D129" s="2" t="n">
         <v>3</v>
@@ -4683,7 +4689,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F130" s="3" t="n">
         <v>3</v>
@@ -4693,7 +4699,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="15" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D131" s="2" t="n">
         <v>3</v>
@@ -4703,7 +4709,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B132" s="1" t="n">
         <v>3</v>
@@ -4713,7 +4719,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B133" s="1" t="n">
         <v>3</v>
@@ -4734,7 +4740,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D136" s="2" t="n">
         <v>3</v>
@@ -4744,7 +4750,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D137" s="2" t="n">
         <v>3</v>
@@ -4754,7 +4760,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F138" s="3" t="n">
         <v>3</v>
@@ -4764,7 +4770,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D139" s="2" t="n">
         <v>3</v>
@@ -4774,7 +4780,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D140" s="2" t="n">
         <v>3</v>
@@ -4788,7 +4794,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D142" s="2" t="n">
         <v>2</v>
@@ -4802,7 +4808,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B144" s="1" t="n">
         <v>2</v>
@@ -4812,7 +4818,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B145" s="1" t="n">
         <v>2</v>
@@ -4822,7 +4828,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="14" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F146" s="3" t="n">
         <v>2</v>
@@ -4832,7 +4838,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B147" s="1" t="n">
         <v>2</v>
@@ -4848,7 +4854,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="15" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D149" s="2" t="n">
         <v>2</v>
@@ -4858,7 +4864,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="14" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F150" s="3" t="n">
         <v>2</v>
@@ -4866,7 +4872,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D151" s="2" t="n">
         <v>2</v>
@@ -4878,7 +4884,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="15" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D153" s="2" t="n">
         <v>2</v>
@@ -4886,7 +4892,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E154" s="14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F154" s="3" t="n">
         <v>2</v>
@@ -4894,7 +4900,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="15" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D155" s="2" t="n">
         <v>2</v>
@@ -4902,7 +4908,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="14" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F156" s="3" t="n">
         <v>2</v>
@@ -4910,7 +4916,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D157" s="2" t="n">
         <v>2</v>
@@ -4918,7 +4924,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E158" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F158" s="3" t="n">
         <v>2</v>
@@ -4928,7 +4934,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D159" s="2" t="n">
         <v>2</v>
@@ -4938,7 +4944,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="15" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D160" s="2" t="n">
         <v>2</v>
@@ -4948,7 +4954,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F161" s="3" t="n">
         <v>2</v>
@@ -4958,7 +4964,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F162" s="3" t="n">
         <v>2</v>
@@ -4968,7 +4974,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="15" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D163" s="2" t="n">
         <v>2</v>
@@ -4982,7 +4988,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D165" s="2" t="n">
         <v>2</v>
@@ -4992,7 +4998,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E166" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F166" s="3" t="n">
         <v>2</v>
@@ -5002,7 +5008,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F167" s="3" t="n">
         <v>2</v>
@@ -5012,7 +5018,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D168" s="2" t="n">
         <v>2</v>
@@ -5022,7 +5028,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E169" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F169" s="3" t="n">
         <v>2</v>
@@ -5032,7 +5038,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="14" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F170" s="3" t="n">
         <v>2</v>
@@ -5042,7 +5048,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D171" s="2" t="n">
         <v>2</v>
@@ -5052,7 +5058,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E172" s="14" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F172" s="3" t="n">
         <v>2</v>
@@ -5062,7 +5068,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E173" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F173" s="3" t="n">
         <v>2</v>
@@ -5076,7 +5082,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D176" s="2" t="n">
         <v>2</v>
@@ -5084,7 +5090,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B177" s="1" t="n">
         <v>2</v>
@@ -5092,7 +5098,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B178" s="1" t="n">
         <v>2</v>
@@ -5100,7 +5106,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D179" s="2" t="n">
         <v>2</v>
@@ -5108,7 +5114,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F180" s="3" t="n">
         <v>2</v>
@@ -5116,7 +5122,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="15" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D181" s="2" t="n">
         <v>2</v>
@@ -5124,7 +5130,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E182" s="14" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F182" s="3" t="n">
         <v>2</v>
@@ -5136,7 +5142,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="15" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D184" s="2" t="n">
         <v>2</v>
@@ -5144,7 +5150,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F186" s="3" t="n">
         <v>2</v>
@@ -5152,7 +5158,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C187" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D187" s="2" t="n">
         <v>2</v>
@@ -5160,7 +5166,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C188" s="15" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D188" s="2" t="n">
         <v>2</v>
@@ -5170,7 +5176,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D189" s="2" t="n">
         <v>2</v>
@@ -5180,7 +5186,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="15" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D190" s="2" t="n">
         <v>2</v>
@@ -5190,7 +5196,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F191" s="3" t="n">
         <v>2</v>
@@ -5200,7 +5206,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C192" s="15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D192" s="2" t="n">
         <v>2</v>
@@ -5210,7 +5216,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D193" s="2" t="n">
         <v>2</v>
@@ -5224,7 +5230,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C195" s="15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D195" s="2" t="n">
         <v>2</v>
@@ -5234,7 +5240,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C196" s="15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D196" s="2" t="n">
         <v>2</v>
@@ -5244,7 +5250,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C197" s="15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D197" s="2" t="n">
         <v>2</v>
@@ -5254,7 +5260,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D198" s="2" t="n">
         <v>2</v>
@@ -5264,7 +5270,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F199" s="3" t="n">
         <v>2</v>
@@ -5280,7 +5286,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C201" s="15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D201" s="2" t="n">
         <v>2</v>
@@ -5290,7 +5296,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C202" s="15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D202" s="2" t="n">
         <v>2</v>
@@ -5300,7 +5306,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C203" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D203" s="2" t="n">
         <v>2</v>
@@ -5314,7 +5320,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D206" s="2" t="n">
         <v>2</v>
@@ -5322,7 +5328,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D207" s="2" t="n">
         <v>2</v>
@@ -5330,7 +5336,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D208" s="2" t="n">
         <v>2</v>
@@ -5338,7 +5344,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B209" s="1" t="n">
         <v>2</v>
@@ -5346,7 +5352,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B210" s="1" t="n">
         <v>2</v>
@@ -5354,7 +5360,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B211" s="1" t="n">
         <v>2</v>
@@ -5362,7 +5368,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B212" s="1" t="n">
         <v>2</v>
@@ -5370,7 +5376,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E213" s="14" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F213" s="3" t="n">
         <v>2</v>
@@ -5378,7 +5384,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B214" s="1" t="n">
         <v>1</v>
@@ -5386,7 +5392,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E215" s="14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F215" s="3" t="n">
         <v>1</v>
@@ -5394,7 +5400,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C216" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D216" s="2" t="n">
         <v>1</v>
@@ -5402,7 +5408,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E217" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F217" s="3" t="n">
         <v>1</v>
@@ -5410,7 +5416,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C218" s="15" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D218" s="2" t="n">
         <v>1</v>
@@ -5422,7 +5428,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B220" s="1" t="n">
         <v>1</v>
@@ -5432,7 +5438,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E221" s="14" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F221" s="3" t="n">
         <v>1</v>
@@ -5442,7 +5448,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C222" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D222" s="2" t="n">
         <v>1</v>
@@ -5452,7 +5458,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C223" s="15" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D223" s="2" t="n">
         <v>1</v>
@@ -5462,7 +5468,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E224" s="14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F224" s="3" t="n">
         <v>1</v>
@@ -5472,7 +5478,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E225" s="14" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F225" s="3" t="n">
         <v>1</v>
@@ -5482,7 +5488,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E226" s="14" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F226" s="3" t="n">
         <v>1</v>
@@ -5492,7 +5498,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B227" s="1" t="n">
         <v>1</v>
@@ -5503,7 +5509,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C228" s="15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D228" s="2" t="n">
         <v>1</v>
@@ -5513,7 +5519,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E229" s="14" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F229" s="3" t="n">
         <v>1</v>
@@ -5527,7 +5533,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C231" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D231" s="2" t="n">
         <v>1</v>
@@ -5537,7 +5543,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E232" s="14" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F232" s="3" t="n">
         <v>1</v>
@@ -5547,7 +5553,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C233" s="15" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D233" s="2" t="n">
         <v>1</v>
@@ -5557,7 +5563,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="12" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B234" s="1" t="n">
         <v>1</v>
@@ -5567,7 +5573,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C235" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D235" s="2" t="n">
         <v>1</v>
@@ -5577,7 +5583,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C236" s="15" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D236" s="2" t="n">
         <v>1</v>
@@ -5591,7 +5597,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E238" s="14" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F238" s="3" t="n">
         <v>1</v>
@@ -5601,7 +5607,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C239" s="15" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D239" s="2" t="n">
         <v>1</v>
@@ -5611,7 +5617,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C240" s="15" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D240" s="2" t="n">
         <v>1</v>
@@ -5621,7 +5627,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E241" s="14" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F241" s="3" t="n">
         <v>1</v>
@@ -5631,7 +5637,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C242" s="15" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D242" s="2" t="n">
         <v>1</v>
@@ -5645,7 +5651,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E244" s="14" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F244" s="3" t="n">
         <v>1</v>
@@ -5659,7 +5665,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C246" s="15" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D246" s="2" t="n">
         <v>1</v>
@@ -5669,7 +5675,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E247" s="14" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F247" s="3" t="n">
         <v>1</v>
@@ -5679,7 +5685,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C248" s="15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D248" s="2" t="n">
         <v>1</v>
@@ -5689,7 +5695,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C249" s="15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D249" s="2" t="n">
         <v>1</v>
@@ -5699,7 +5705,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C250" s="15" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D250" s="2" t="n">
         <v>1</v>
@@ -5709,7 +5715,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C251" s="15" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D251" s="2" t="n">
         <v>1</v>
@@ -5719,7 +5725,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C252" s="15" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D252" s="2" t="n">
         <v>1</v>
@@ -5729,7 +5735,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E253" s="14" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F253" s="3" t="n">
         <v>1</v>
@@ -5739,7 +5745,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C254" s="15" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D254" s="2" t="n">
         <v>1</v>
@@ -5749,7 +5755,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E255" s="14" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F255" s="3" t="n">
         <v>1</v>
@@ -5759,7 +5765,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C256" s="15" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D256" s="2" t="n">
         <v>1</v>
@@ -5769,7 +5775,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C257" s="15" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D257" s="2" t="n">
         <v>1</v>
@@ -5781,7 +5787,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C259" s="15" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D259" s="2" t="n">
         <v>1</v>
@@ -5789,7 +5795,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="12" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B260" s="1" t="n">
         <v>1</v>
@@ -5797,7 +5803,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B261" s="1" t="n">
         <v>1</v>
@@ -5805,7 +5811,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B262" s="1" t="n">
         <v>1</v>
@@ -5813,7 +5819,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C263" s="15" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D263" s="2" t="n">
         <v>1</v>
@@ -5821,7 +5827,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="12" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B264" s="1" t="n">
         <v>1</v>
@@ -5829,7 +5835,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C265" s="15" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D265" s="2" t="n">
         <v>1</v>
@@ -5841,7 +5847,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E267" s="14" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F267" s="3" t="n">
         <v>1</v>
@@ -5851,7 +5857,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C268" s="15" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D268" s="2" t="n">
         <v>1</v>
@@ -5861,7 +5867,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E269" s="14" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F269" s="3" t="n">
         <v>1</v>
@@ -5871,7 +5877,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C270" s="15" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D270" s="2" t="n">
         <v>1</v>
@@ -5881,7 +5887,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B271" s="1" t="n">
         <v>1</v>
@@ -5891,7 +5897,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B272" s="1" t="n">
         <v>1</v>
@@ -5901,7 +5907,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E273" s="14" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F273" s="3" t="n">
         <v>1</v>
@@ -5915,7 +5921,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C275" s="15" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D275" s="2" t="n">
         <v>1</v>
@@ -5925,7 +5931,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C276" s="15" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D276" s="2" t="n">
         <v>1</v>
@@ -5935,7 +5941,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E277" s="14" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F277" s="3" t="n">
         <v>1</v>
@@ -5945,7 +5951,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C278" s="15" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D278" s="2" t="n">
         <v>1</v>
@@ -5955,7 +5961,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E279" s="14" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F279" s="3" t="n">
         <v>1</v>
@@ -5969,7 +5975,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E281" s="14" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F281" s="3" t="n">
         <v>1</v>
@@ -5983,7 +5989,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B283" s="1" t="n">
         <v>1</v>
@@ -5993,7 +5999,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E284" s="14" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F284" s="3" t="n">
         <v>1</v>
@@ -6003,7 +6009,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C285" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D285" s="2" t="n">
         <v>1</v>
@@ -6013,7 +6019,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="12" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B286" s="1" t="n">
         <v>1</v>
@@ -6023,7 +6029,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E287" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F287" s="3" t="n">
         <v>1</v>
@@ -6033,7 +6039,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E288" s="14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F288" s="3" t="n">
         <v>1</v>
@@ -6043,7 +6049,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C289" s="15" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D289" s="2" t="n">
         <v>1</v>
@@ -6053,7 +6059,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="12" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B290" s="1" t="n">
         <v>1</v>
@@ -6063,7 +6069,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C291" s="15" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D291" s="2" t="n">
         <v>1</v>
@@ -6073,7 +6079,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C292" s="15" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D292" s="2" t="n">
         <v>1</v>
@@ -6083,7 +6089,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C293" s="15" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D293" s="2" t="n">
         <v>1</v>
@@ -6091,7 +6097,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C294" s="15" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D294" s="2" t="n">
         <v>1</v>
@@ -6099,7 +6105,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C295" s="15" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D295" s="2" t="n">
         <v>1</v>
@@ -6107,7 +6113,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C296" s="15" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D296" s="2" t="n">
         <v>1</v>
@@ -6115,7 +6121,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C297" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D297" s="2" t="n">
         <v>1</v>
@@ -6123,7 +6129,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E298" s="14" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F298" s="3" t="n">
         <v>1</v>
@@ -6131,7 +6137,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C299" s="15" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D299" s="2" t="n">
         <v>1</v>
@@ -6139,7 +6145,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C300" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D300" s="2" t="n">
         <v>1</v>
@@ -6147,7 +6153,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C301" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D301" s="2" t="n">
         <v>1</v>
@@ -6167,7 +6173,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="12" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B304" s="1" t="n">
         <v>1</v>
@@ -6177,7 +6183,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C305" s="15" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D305" s="2" t="n">
         <v>1</v>
@@ -6187,7 +6193,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C306" s="15" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D306" s="2" t="n">
         <v>1</v>
@@ -6205,7 +6211,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C309" s="15" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D309" s="2" t="n">
         <v>1</v>
@@ -6215,7 +6221,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B310" s="1" t="n">
         <v>1</v>
@@ -6223,7 +6229,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B311" s="1" t="n">
         <v>1</v>
@@ -6231,7 +6237,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C312" s="15" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D312" s="2" t="n">
         <v>1</v>
@@ -6239,7 +6245,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C313" s="15" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D313" s="2" t="n">
         <v>1</v>
@@ -6248,7 +6254,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E314" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F314" s="3" t="n">
         <v>1</v>
@@ -6256,7 +6262,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E315" s="14" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F315" s="3" t="n">
         <v>1</v>
@@ -6264,7 +6270,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C316" s="15" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D316" s="2" t="n">
         <v>1</v>
@@ -6272,7 +6278,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C317" s="15" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D317" s="2" t="n">
         <v>1</v>
@@ -6280,7 +6286,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C318" s="15" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D318" s="2" t="n">
         <v>1</v>
@@ -6288,7 +6294,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="12" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B319" s="1" t="n">
         <v>1</v>
@@ -6296,7 +6302,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C320" s="15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D320" s="2" t="n">
         <v>1</v>
@@ -6305,7 +6311,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E321" s="14" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F321" s="3" t="n">
         <v>1</v>
@@ -6313,7 +6319,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C322" s="15" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D322" s="2" t="n">
         <v>1</v>
@@ -6321,7 +6327,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B323" s="1" t="n">
         <v>1</v>
@@ -6333,7 +6339,7 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="12" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B325" s="1" t="n">
         <v>1</v>
@@ -6343,7 +6349,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C326" s="15" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D326" s="2" t="n">
         <v>1</v>
@@ -6353,7 +6359,7 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E327" s="14" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F327" s="3" t="n">
         <v>1</v>
@@ -6363,7 +6369,7 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E328" s="15" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F328" s="2" t="n">
         <v>1</v>
@@ -6377,7 +6383,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C330" s="15" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D330" s="2" t="n">
         <v>1</v>
@@ -6387,7 +6393,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E331" s="14" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F331" s="3" t="n">
         <v>1</v>
@@ -6397,7 +6403,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C332" s="15" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D332" s="2" t="n">
         <v>1</v>
@@ -6407,7 +6413,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="12" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B333" s="1" t="n">
         <v>1</v>
@@ -6415,7 +6421,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C334" s="15" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D334" s="2" t="n">
         <v>1</v>
@@ -6423,7 +6429,7 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C335" s="15" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D335" s="2" t="n">
         <v>1</v>
@@ -6435,7 +6441,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C337" s="15" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D337" s="2" t="n">
         <v>1</v>
@@ -6445,7 +6451,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C338" s="15" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D338" s="2" t="n">
         <v>1</v>
@@ -6455,7 +6461,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C339" s="15" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D339" s="2" t="n">
         <v>1</v>
@@ -6465,7 +6471,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C340" s="15" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D340" s="2" t="n">
         <v>1</v>
@@ -6476,7 +6482,7 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E341" s="14" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F341" s="3" t="n">
         <v>1</v>
@@ -6486,7 +6492,7 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E342" s="14" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F342" s="3" t="n">
         <v>1</v>
@@ -6496,7 +6502,7 @@
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C343" s="15" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D343" s="2" t="n">
         <v>1</v>
@@ -6506,7 +6512,7 @@
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C344" s="15" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D344" s="2" t="n">
         <v>1</v>
@@ -6514,7 +6520,7 @@
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B345" s="1" t="n">
         <v>1</v>
@@ -6522,7 +6528,7 @@
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C346" s="15" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D346" s="2" t="n">
         <v>1</v>
@@ -6530,7 +6536,7 @@
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E347" s="14" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F347" s="3" t="n">
         <v>1</v>
@@ -6538,7 +6544,7 @@
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B348" s="1" t="n">
         <v>1</v>
@@ -6546,7 +6552,7 @@
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C349" s="15" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D349" s="2" t="n">
         <v>1</v>
@@ -6554,7 +6560,7 @@
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C350" s="15" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D350" s="2" t="n">
         <v>1</v>
@@ -6562,7 +6568,7 @@
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E351" s="14" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F351" s="3" t="n">
         <v>1</v>
@@ -6570,7 +6576,7 @@
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E352" s="14" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F352" s="3" t="n">
         <v>1</v>
@@ -6578,7 +6584,7 @@
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E353" s="14" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F353" s="3" t="n">
         <v>1</v>
@@ -6591,7 +6597,7 @@
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C355" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D355" s="2" t="n">
         <v>1</v>
@@ -6601,7 +6607,7 @@
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E356" s="14" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F356" s="3" t="n">
         <v>1</v>
@@ -6611,7 +6617,7 @@
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C357" s="15" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D357" s="2" t="n">
         <v>1</v>
@@ -6621,7 +6627,7 @@
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E358" s="14" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F358" s="3" t="n">
         <v>1</v>
@@ -6631,7 +6637,7 @@
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E359" s="14" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F359" s="3" t="n">
         <v>1</v>
@@ -6641,7 +6647,7 @@
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C360" s="15" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D360" s="2" t="n">
         <v>1</v>
@@ -6651,7 +6657,7 @@
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E361" s="14" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F361" s="3" t="n">
         <v>1</v>
@@ -6660,7 +6666,7 @@
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E362" s="14" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F362" s="3" t="n">
         <v>1</v>
@@ -6672,7 +6678,7 @@
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C364" s="15" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D364" s="2" t="n">
         <v>1</v>
@@ -6682,7 +6688,7 @@
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C365" s="15" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D365" s="2" t="n">
         <v>1</v>
@@ -6693,7 +6699,7 @@
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C366" s="15" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D366" s="2" t="n">
         <v>1</v>
@@ -6704,7 +6710,7 @@
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E367" s="14" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F367" s="3" t="n">
         <v>1</v>
@@ -6720,7 +6726,7 @@
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C369" s="15" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D369" s="2" t="n">
         <v>1</v>
@@ -6728,7 +6734,7 @@
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C370" s="15" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D370" s="2" t="n">
         <v>1</v>
@@ -6736,7 +6742,7 @@
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C371" s="15" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D371" s="2" t="n">
         <v>1</v>
@@ -6748,7 +6754,7 @@
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C373" s="15" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D373" s="2" t="n">
         <v>1</v>
@@ -6756,7 +6762,7 @@
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C374" s="15" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D374" s="2" t="n">
         <v>1</v>
@@ -6764,7 +6770,7 @@
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C375" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D375" s="2" t="n">
         <v>1</v>
@@ -6772,13 +6778,13 @@
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C376" s="15" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D376" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E376" s="14" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F376" s="3" t="n">
         <v>1</v>
@@ -6786,7 +6792,7 @@
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E377" s="14" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F377" s="3" t="n">
         <v>1</v>
@@ -6794,7 +6800,7 @@
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C378" s="15" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D378" s="2" t="n">
         <v>1</v>
@@ -6802,7 +6808,7 @@
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E379" s="14" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F379" s="3" t="n">
         <v>1</v>
@@ -6810,7 +6816,7 @@
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C380" s="15" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D380" s="2" t="n">
         <v>1</v>
@@ -6818,7 +6824,7 @@
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E381" s="14" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F381" s="3" t="n">
         <v>1</v>
@@ -6826,7 +6832,7 @@
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C382" s="15" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D382" s="2" t="n">
         <v>1</v>
@@ -6834,7 +6840,7 @@
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C383" s="15" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D383" s="2" t="n">
         <v>1</v>
@@ -6842,7 +6848,7 @@
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E384" s="14" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F384" s="3" t="n">
         <v>1</v>
@@ -6850,7 +6856,7 @@
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C385" s="15" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D385" s="2" t="n">
         <v>1</v>
@@ -6858,7 +6864,7 @@
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C386" s="15" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D386" s="2" t="n">
         <v>1</v>
@@ -6866,7 +6872,7 @@
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C387" s="15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D387" s="2" t="n">
         <v>1</v>
@@ -6874,7 +6880,7 @@
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C388" s="15" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D388" s="2" t="n">
         <v>1</v>
@@ -6882,7 +6888,7 @@
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C389" s="15" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D389" s="2" t="n">
         <v>1</v>
@@ -6894,7 +6900,7 @@
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C390" s="15" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D390" s="2" t="n">
         <v>1</v>
@@ -6906,7 +6912,7 @@
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E391" s="15" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F391" s="2" t="n">
         <v>1</v>
@@ -6916,7 +6922,7 @@
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C392" s="15" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D392" s="2" t="n">
         <v>1</v>
@@ -6926,7 +6932,7 @@
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C393" s="15" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D393" s="2" t="n">
         <v>1</v>
@@ -6936,7 +6942,7 @@
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C394" s="15" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D394" s="2" t="n">
         <v>1</v>
@@ -6944,7 +6950,7 @@
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C395" s="15" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D395" s="2" t="n">
         <v>1</v>
@@ -6952,7 +6958,7 @@
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C396" s="15" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D396" s="2" t="n">
         <v>1</v>
@@ -6960,7 +6966,7 @@
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C397" s="15" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D397" s="2" t="n">
         <v>1</v>
@@ -6968,7 +6974,7 @@
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C398" s="15" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D398" s="2" t="n">
         <v>1</v>
@@ -6976,7 +6982,7 @@
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C399" s="15" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D399" s="2" t="n">
         <v>1</v>
@@ -6984,7 +6990,7 @@
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C400" s="15" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D400" s="2" t="n">
         <v>1</v>
@@ -6992,7 +6998,7 @@
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C401" s="15" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D401" s="2" t="n">
         <v>1</v>
@@ -7000,7 +7006,7 @@
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E402" s="14" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F402" s="3" t="n">
         <v>1</v>
@@ -7008,7 +7014,7 @@
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C403" s="15" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D403" s="2" t="n">
         <v>1</v>
@@ -7018,7 +7024,7 @@
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C405" s="15" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D405" s="2" t="n">
         <v>1</v>
@@ -7026,7 +7032,7 @@
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C406" s="15" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D406" s="2" t="n">
         <v>1</v>
@@ -7034,7 +7040,7 @@
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C407" s="15" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D407" s="2" t="n">
         <v>1</v>
@@ -7042,7 +7048,7 @@
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C408" s="15" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D408" s="2" t="n">
         <v>1</v>
@@ -7050,7 +7056,7 @@
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C409" s="15" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D409" s="2" t="n">
         <v>1</v>
@@ -7058,7 +7064,7 @@
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C410" s="15" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D410" s="2" t="n">
         <v>1</v>
@@ -7066,7 +7072,7 @@
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C411" s="15" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D411" s="2" t="n">
         <v>1</v>
@@ -7074,7 +7080,7 @@
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C412" s="15" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D412" s="2" t="n">
         <v>1</v>
@@ -7082,7 +7088,7 @@
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C413" s="15" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D413" s="2" t="n">
         <v>1</v>
@@ -7094,7 +7100,7 @@
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C416" s="15" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D416" s="2" t="n">
         <v>1</v>
@@ -7106,7 +7112,7 @@
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C418" s="15" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D418" s="2" t="n">
         <v>1</v>
@@ -7116,7 +7122,7 @@
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C419" s="15" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D419" s="2" t="n">
         <v>1</v>
@@ -7130,7 +7136,7 @@
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C421" s="15" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D421" s="2" t="n">
         <v>1</v>
@@ -7140,7 +7146,7 @@
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C422" s="15" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D422" s="2" t="n">
         <v>1</v>
@@ -7148,7 +7154,7 @@
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C423" s="15" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D423" s="2" t="n">
         <v>1</v>
@@ -7156,7 +7162,7 @@
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C424" s="15" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D424" s="2" t="n">
         <v>1</v>
@@ -7164,7 +7170,7 @@
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="12" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B425" s="1" t="n">
         <v>1</v>
@@ -7172,7 +7178,7 @@
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C426" s="15" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D426" s="2" t="n">
         <v>1</v>
@@ -7180,7 +7186,7 @@
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C427" s="15" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D427" s="2" t="n">
         <v>1</v>
@@ -7188,7 +7194,7 @@
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C428" s="15" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D428" s="2" t="n">
         <v>1</v>
@@ -7196,19 +7202,15 @@
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C429" s="15" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D429" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="D430" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="C430" s="0"/>
+      <c r="D430" s="0"/>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C431" s="15" t="s">

</xml_diff>

<commit_message>
Update task 4 to NACE categories
</commit_message>
<xml_diff>
--- a/src/team_4/tokens_dict.xlsx
+++ b/src/team_4/tokens_dict.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">פנסיונר</t>
   </si>
   <si>
-    <t xml:space="preserve">לא\s?</t>
+    <t xml:space="preserve">לא</t>
   </si>
   <si>
     <t xml:space="preserve">על </t>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">מצבו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מובטל</t>
   </si>
   <si>
     <t xml:space="preserve">גימלאית</t>
@@ -317,9 +320,6 @@
     <t xml:space="preserve">בפנסיה</t>
   </si>
   <si>
-    <t xml:space="preserve">מובטל</t>
-  </si>
-  <si>
     <t xml:space="preserve">בת</t>
   </si>
   <si>
@@ -383,103 +383,103 @@
     <t xml:space="preserve">ילדים</t>
   </si>
   <si>
+    <t xml:space="preserve">מטפלת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">איש</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מזכירה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חשבונות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מרכז</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בתחום</t>
+  </si>
+  <si>
+    <t xml:space="preserve">טכנאי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חברת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חברה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פקידה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ספר</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גננת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">במשרד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סייעת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">עלו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מרצה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">צרפתי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בגן</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בלוונשטיין</t>
+  </si>
+  <si>
+    <t xml:space="preserve">דיאליזה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חנות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בחברת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פינסונרית</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בעלת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בארקיע</t>
+  </si>
+  <si>
     <t xml:space="preserve">בעל</t>
   </si>
   <si>
-    <t xml:space="preserve">מטפלת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">איש</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מזכירה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בעלת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">חשבונות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מרכז</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בתחום</t>
-  </si>
-  <si>
-    <t xml:space="preserve">טכנאי</t>
-  </si>
-  <si>
-    <t xml:space="preserve">חברת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">חברה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">פקידה</t>
+    <t xml:space="preserve">בדימונה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חשמלאי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לווינשטיין</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מחשבים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מהשתלת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">משאית</t>
   </si>
   <si>
     <t xml:space="preserve">ניהול</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ספר</t>
-  </si>
-  <si>
-    <t xml:space="preserve">גננת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">במשרד</t>
-  </si>
-  <si>
-    <t xml:space="preserve">סייעת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">עלו</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מרצה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">צרפתי</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בגן</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בלוונשטיין</t>
-  </si>
-  <si>
-    <t xml:space="preserve">דיאליזה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">חנות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בחברת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">פינסונרית</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בארקיע</t>
-  </si>
-  <si>
-    <t xml:space="preserve">בדימונה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">חשמלאי</t>
-  </si>
-  <si>
-    <t xml:space="preserve">לווינשטיין</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מחשבים</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מהשתלת</t>
-  </si>
-  <si>
-    <t xml:space="preserve">משאית</t>
   </si>
   <si>
     <t xml:space="preserve">מוגבל</t>
@@ -531,6 +531,9 @@
     <t xml:space="preserve">אגד</t>
   </si>
   <si>
+    <t xml:space="preserve">משרד</t>
+  </si>
+  <si>
     <t xml:space="preserve">הרצליה</t>
   </si>
   <si>
@@ -541,9 +544,6 @@
   </si>
   <si>
     <t xml:space="preserve">מסגר</t>
-  </si>
-  <si>
-    <t xml:space="preserve">משרד</t>
   </si>
   <si>
     <t xml:space="preserve">שפיים</t>
@@ -2919,8 +2919,8 @@
   </sheetPr>
   <dimension ref="A1:L645"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O84" activeCellId="0" sqref="O84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3126,12 +3126,18 @@
       <c r="H9" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="K9" s="11"/>
       <c r="L9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>88</v>
@@ -3139,7 +3145,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="K10" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L10" s="9" t="n">
         <v>25</v>
@@ -3147,19 +3153,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>84</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H11" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L11" s="9" t="n">
         <v>24</v>
@@ -3167,19 +3173,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>75</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H12" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L12" s="9" t="n">
         <v>22</v>
@@ -3187,19 +3193,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>2</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H13" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L13" s="9" t="n">
         <v>17</v>
@@ -3207,7 +3213,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>51</v>
@@ -3215,13 +3221,13 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="G14" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H14" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L14" s="9" t="n">
         <v>15</v>
@@ -3229,25 +3235,25 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L15" s="9" t="n">
         <v>12</v>
@@ -3255,13 +3261,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>47</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L16" s="9" t="n">
         <v>8</v>
@@ -3269,13 +3275,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>46</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L17" s="9" t="n">
         <v>7</v>
@@ -3283,19 +3289,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>37</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>70</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L18" s="9" t="n">
         <v>4</v>
@@ -3303,13 +3309,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>34</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L19" s="9" t="n">
         <v>3</v>
@@ -3317,7 +3323,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>27</v>
@@ -3325,7 +3331,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L20" s="9" t="n">
         <v>2</v>
@@ -3333,7 +3339,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>27</v>
@@ -3341,7 +3347,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L21" s="9" t="n">
         <v>2</v>
@@ -3352,7 +3358,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L22" s="9" t="n">
         <v>2</v>
@@ -3360,7 +3366,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K23" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L23" s="9" t="n">
         <v>1</v>
@@ -3372,7 +3378,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L24" s="9" t="n">
         <v>1</v>
@@ -3383,7 +3389,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L25" s="9" t="n">
         <v>1</v>
@@ -3391,7 +3397,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>20</v>
@@ -3399,7 +3405,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L26" s="9" t="n">
         <v>1</v>
@@ -3407,7 +3413,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F27" s="3" t="n">
         <v>19</v>
@@ -3415,7 +3421,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L27" s="9" t="n">
         <v>1</v>
@@ -3423,7 +3429,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>19</v>
@@ -3431,7 +3437,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L28" s="9" t="n">
         <v>1</v>
@@ -3439,7 +3445,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>18</v>
@@ -3447,27 +3453,21 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L29" s="9" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F30" s="3" t="n">
-        <v>3</v>
-      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="11" t="s">
@@ -3651,16 +3651,12 @@
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="L43" s="14" t="n">
-        <v>7</v>
-      </c>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>10</v>
@@ -3668,7 +3664,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
       <c r="K44" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L44" s="14" t="n">
         <v>7</v>
@@ -3676,23 +3672,19 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F45" s="3" t="n">
         <v>9</v>
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="L45" s="3" t="n">
-        <v>4</v>
-      </c>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D46" s="2" t="n">
         <v>9</v>
@@ -3700,7 +3692,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L46" s="3" t="n">
         <v>1</v>
@@ -3712,7 +3704,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L47" s="2" t="n">
         <v>3</v>
@@ -3720,7 +3712,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F48" s="3" t="n">
         <v>9</v>
@@ -3728,7 +3720,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
       <c r="K48" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L48" s="2" t="n">
         <v>4</v>
@@ -3738,7 +3730,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
       <c r="K49" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L49" s="2" t="n">
         <v>4</v>
@@ -3746,29 +3738,25 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F50" s="3" t="n">
         <v>8</v>
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="L50" s="2" t="n">
-        <v>2</v>
-      </c>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D51" s="14" t="n">
         <v>7</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F51" s="3" t="n">
         <v>8</v>
@@ -3776,7 +3764,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L51" s="2" t="n">
         <v>2</v>
@@ -3784,7 +3772,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F52" s="14" t="n">
         <v>8</v>
@@ -3792,7 +3780,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
       <c r="K52" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L52" s="2" t="n">
         <v>1</v>
@@ -3800,7 +3788,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F53" s="14" t="n">
         <v>8</v>
@@ -3808,7 +3796,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
       <c r="K53" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L53" s="2" t="n">
         <v>1</v>
@@ -3816,7 +3804,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D54" s="2" t="n">
         <v>8</v>
@@ -3826,7 +3814,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
       <c r="K54" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="L54" s="2" t="n">
         <v>1</v>
@@ -3838,7 +3826,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
       <c r="K55" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L55" s="2" t="n">
         <v>1</v>
@@ -3846,7 +3834,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D56" s="2" t="n">
         <v>7</v>
@@ -3856,7 +3844,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
       <c r="K56" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L56" s="2" t="n">
         <v>1</v>
@@ -3864,29 +3852,37 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
+      <c r="E57" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
       <c r="K57" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L57" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="E58" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F58" s="14" t="n">
+        <v>7</v>
+      </c>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
       <c r="K58" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L58" s="2" t="n">
         <v>1</v>
@@ -3894,7 +3890,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F59" s="14" t="n">
         <v>7</v>
@@ -3902,7 +3898,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
       <c r="K59" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L59" s="2" t="n">
         <v>1</v>
@@ -3910,7 +3906,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D60" s="2" t="n">
         <v>7</v>
@@ -3920,7 +3916,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
       <c r="K60" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L60" s="2" t="n">
         <v>1</v>
@@ -3928,13 +3924,17 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D61" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="E61" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F61" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
       <c r="K61" s="15" t="s">
@@ -4023,12 +4023,16 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="E67" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <v>7</v>
+      </c>
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
       <c r="K67" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L67" s="2" t="n">
         <v>1</v>
@@ -4036,7 +4040,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="14" t="n">
         <v>6</v>
@@ -4046,7 +4050,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
       <c r="K68" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L68" s="2" t="n">
         <v>1</v>
@@ -4054,19 +4058,15 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F69" s="14" t="n">
         <v>6</v>
       </c>
       <c r="I69" s="8"/>
       <c r="J69" s="8"/>
-      <c r="K69" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="L69" s="2" t="n">
-        <v>7</v>
-      </c>
+      <c r="K69" s="0"/>
+      <c r="L69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="14"/>
@@ -7209,8 +7209,8 @@
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="0"/>
-      <c r="D430" s="0"/>
+      <c r="C430" s="6"/>
+      <c r="D430" s="6"/>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C431" s="15" t="s">

</xml_diff>